<commit_message>
add functions of radio button
</commit_message>
<xml_diff>
--- a/Actualizacion de datos/PRUEBA DE ESCRITORIO.xlsx
+++ b/Actualizacion de datos/PRUEBA DE ESCRITORIO.xlsx
@@ -1,18 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ftorrenegra/Desktop/Simulador/Actualizacion de datos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="-28000" yWindow="-12940" windowWidth="24420" windowHeight="14720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="interfaz gráfica" sheetId="1" r:id="rId1"/>
     <sheet name="Prueba de escritorio" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="134">
   <si>
     <t>Conexión</t>
   </si>
@@ -947,6 +958,9 @@
   </si>
   <si>
     <t>VT</t>
+  </si>
+  <si>
+    <t>Deltas</t>
   </si>
 </sst>
 </file>
@@ -1099,26 +1113,26 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1126,17 +1140,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1146,7 +1160,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1154,36 +1168,36 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1191,35 +1205,35 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1228,17 +1242,17 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1249,7 +1263,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1319,6 +1333,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1355,26 +1370,17 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1403,7 +1409,15 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2880,7 +2894,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2890,39 +2904,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AG36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.140625" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="3.5" customWidth="1"/>
+    <col min="11" max="11" width="3.1640625" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.1640625" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.1640625" customWidth="1"/>
     <col min="19" max="20" width="3" customWidth="1"/>
-    <col min="21" max="21" width="3.140625" customWidth="1"/>
+    <col min="21" max="21" width="3.1640625" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
-    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.7109375" customWidth="1"/>
-    <col min="26" max="26" width="3.5703125" customWidth="1"/>
-    <col min="27" max="27" width="4.42578125" customWidth="1"/>
-    <col min="31" max="31" width="6.5703125" customWidth="1"/>
-    <col min="32" max="32" width="3.5703125" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.6640625" customWidth="1"/>
+    <col min="26" max="26" width="3.5" customWidth="1"/>
+    <col min="27" max="27" width="4.5" customWidth="1"/>
+    <col min="31" max="31" width="6.5" customWidth="1"/>
+    <col min="32" max="32" width="3.5" customWidth="1"/>
     <col min="33" max="33" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -2956,43 +2970,43 @@
       <c r="AF2" s="12"/>
       <c r="AG2" s="12"/>
     </row>
-    <row r="3" spans="2:33" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:33" ht="26" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="34"/>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="34"/>
-      <c r="AE3" s="34"/>
-      <c r="AF3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
       <c r="AG3" s="12"/>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -3026,7 +3040,7 @@
       <c r="AF4" s="12"/>
       <c r="AG4" s="12"/>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -3060,18 +3074,18 @@
       <c r="AF5" s="6"/>
       <c r="AG5" s="12"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -3083,24 +3097,24 @@
       <c r="S6" s="6"/>
       <c r="T6" s="12"/>
       <c r="U6" s="6"/>
-      <c r="V6" s="33" t="s">
+      <c r="V6" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="W6" s="33"/>
-      <c r="X6" s="33"/>
-      <c r="Y6" s="33"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="35" t="s">
+      <c r="AA6" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="AB6" s="36"/>
-      <c r="AC6" s="36"/>
-      <c r="AD6" s="36"/>
-      <c r="AE6" s="37"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="37"/>
+      <c r="AE6" s="38"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="12"/>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -3134,7 +3148,7 @@
       <c r="AF7" s="6"/>
       <c r="AG7" s="12"/>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
@@ -3168,7 +3182,7 @@
       <c r="AF8" s="6"/>
       <c r="AG8" s="12"/>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
@@ -3210,7 +3224,7 @@
       <c r="AF9" s="6"/>
       <c r="AG9" s="12"/>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
@@ -3244,7 +3258,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="12"/>
     </row>
-    <row r="11" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
@@ -3296,7 +3310,7 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="12"/>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
@@ -3330,7 +3344,7 @@
       <c r="AF12" s="6"/>
       <c r="AG12" s="12"/>
     </row>
-    <row r="13" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
@@ -3376,7 +3390,7 @@
       <c r="AF13" s="6"/>
       <c r="AG13" s="12"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="C14" s="6"/>
       <c r="D14" s="2"/>
@@ -3410,7 +3424,7 @@
       <c r="AF14" s="6"/>
       <c r="AG14" s="12"/>
     </row>
-    <row r="15" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
@@ -3458,7 +3472,7 @@
       <c r="AF15" s="6"/>
       <c r="AG15" s="12"/>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
@@ -3492,7 +3506,7 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="12"/>
     </row>
-    <row r="17" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
@@ -3546,7 +3560,7 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="12"/>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
@@ -3580,7 +3594,7 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="12"/>
     </row>
-    <row r="19" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
@@ -3591,10 +3605,10 @@
         <v>60</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="38" t="s">
+      <c r="H19" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="39"/>
+      <c r="I19" s="40"/>
       <c r="J19" s="2"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -3624,15 +3638,15 @@
       <c r="AF19" s="6"/>
       <c r="AG19" s="12"/>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="3"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="2"/>
       <c r="K20" s="6"/>
       <c r="L20" s="7"/>
@@ -3658,7 +3672,7 @@
       <c r="AF20" s="6"/>
       <c r="AG20" s="12"/>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
@@ -3669,8 +3683,8 @@
         <v>0.8</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44"/>
       <c r="J21" s="2"/>
       <c r="K21" s="6"/>
       <c r="L21" s="7"/>
@@ -3702,7 +3716,7 @@
       <c r="AF21" s="6"/>
       <c r="AG21" s="12"/>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
@@ -3736,7 +3750,7 @@
       <c r="AF22" s="6"/>
       <c r="AG22" s="12"/>
     </row>
-    <row r="23" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -3778,7 +3792,7 @@
       <c r="AF23" s="6"/>
       <c r="AG23" s="12"/>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
@@ -3812,7 +3826,7 @@
       <c r="AF24" s="6"/>
       <c r="AG24" s="12"/>
     </row>
-    <row r="25" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -3856,7 +3870,7 @@
       <c r="AF25" s="6"/>
       <c r="AG25" s="12"/>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -3890,7 +3904,7 @@
       <c r="AF26" s="6"/>
       <c r="AG26" s="12"/>
     </row>
-    <row r="27" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -3928,7 +3942,7 @@
       <c r="AF27" s="6"/>
       <c r="AG27" s="12"/>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
@@ -3962,7 +3976,7 @@
       <c r="AF28" s="6"/>
       <c r="AG28" s="12"/>
     </row>
-    <row r="29" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
@@ -4008,7 +4022,7 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="12"/>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
@@ -4042,7 +4056,7 @@
       <c r="AF30" s="6"/>
       <c r="AG30" s="12"/>
     </row>
-    <row r="31" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
@@ -4080,7 +4094,7 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="12"/>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
@@ -4114,7 +4128,7 @@
       <c r="AF32" s="6"/>
       <c r="AG32" s="12"/>
     </row>
-    <row r="33" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:33" ht="17" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
@@ -4164,7 +4178,7 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="12"/>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B34" s="12"/>
       <c r="C34" s="6"/>
       <c r="D34" s="7"/>
@@ -4198,7 +4212,7 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="12"/>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B35" s="12"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -4232,7 +4246,7 @@
       <c r="AF35" s="6"/>
       <c r="AG35" s="12"/>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -4283,34 +4297,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="86" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="3" style="19" customWidth="1"/>
-    <col min="3" max="8" width="11.42578125" style="19"/>
-    <col min="9" max="9" width="12.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" style="19" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" style="19" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="19"/>
-    <col min="17" max="17" width="13.7109375" style="19" customWidth="1"/>
+    <col min="3" max="8" width="10.83203125" style="19"/>
+    <col min="9" max="9" width="12.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="3.5" style="19" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="19"/>
+    <col min="17" max="17" width="13.6640625" style="19" customWidth="1"/>
     <col min="18" max="18" width="6" style="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="11.42578125" style="19"/>
-    <col min="22" max="22" width="16.28515625" style="19" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="19"/>
-    <col min="24" max="24" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="10.83203125" style="19"/>
+    <col min="22" max="22" width="16.33203125" style="19" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="19"/>
+    <col min="24" max="24" width="14.83203125" style="19" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="11.42578125" style="19"/>
+    <col min="26" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -4323,51 +4337,51 @@
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
       <c r="M2" s="18"/>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="49"/>
-      <c r="V2" s="47" t="s">
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
+      <c r="V2" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="49"/>
-    </row>
-    <row r="3" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="61"/>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
       <c r="M3" s="21"/>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="21"/>
-      <c r="V3" s="45" t="s">
+      <c r="V3" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="Y3" s="22"/>
       <c r="Z3" s="22"/>
       <c r="AA3" s="21"/>
@@ -4414,18 +4428,18 @@
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
       <c r="M5" s="21"/>
       <c r="O5" s="20" t="s">
         <v>74</v>
@@ -4456,18 +4470,18 @@
       <c r="Z5" s="22"/>
       <c r="AA5" s="21"/>
     </row>
-    <row r="6" spans="2:27" ht="19.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B6" s="20"/>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="55" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="57" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="23" t="s">
@@ -4485,7 +4499,7 @@
       <c r="K6" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="57" t="s">
+      <c r="L6" s="55" t="s">
         <v>2</v>
       </c>
       <c r="M6" s="21"/>
@@ -4518,12 +4532,12 @@
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B7" s="20"/>
-      <c r="C7" s="58"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="60"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="24" t="s">
         <v>50</v>
       </c>
@@ -4537,7 +4551,7 @@
       <c r="K7" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="58"/>
+      <c r="L7" s="56"/>
       <c r="M7" s="21"/>
       <c r="O7" s="20"/>
       <c r="P7" s="22" t="s">
@@ -4545,7 +4559,7 @@
       </c>
       <c r="Q7" s="22">
         <f>IF(J8="Delta",D8,D8/SQRT(3))</f>
-        <v>220</v>
+        <v>127.01705922171767</v>
       </c>
       <c r="R7" s="22" t="s">
         <v>86</v>
@@ -4587,7 +4601,7 @@
         <v>0.8</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="K8" s="25">
         <v>60</v>
@@ -4614,7 +4628,7 @@
       <c r="Z8" s="22"/>
       <c r="AA8" s="21"/>
     </row>
-    <row r="9" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -4627,11 +4641,11 @@
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
       <c r="M9" s="21"/>
-      <c r="O9" s="45" t="s">
+      <c r="O9" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="21"/>
@@ -4649,17 +4663,17 @@
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B10" s="20"/>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="K10" s="52" t="s">
+      <c r="K10" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="53"/>
+      <c r="L10" s="51"/>
       <c r="M10" s="21"/>
       <c r="O10" s="20" t="s">
         <v>62</v>
@@ -4733,7 +4747,7 @@
       </c>
       <c r="X11" s="22">
         <f>IF(J8="Delta",X10,D8/SQRT(3))</f>
-        <v>220.02697302174033</v>
+        <v>127.01705922171767</v>
       </c>
       <c r="Y11" s="22" t="s">
         <v>86</v>
@@ -4783,7 +4797,7 @@
       <c r="Z12" s="22"/>
       <c r="AA12" s="21"/>
     </row>
-    <row r="13" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B13" s="20"/>
       <c r="C13" s="28">
         <v>0.25</v>
@@ -4806,16 +4820,16 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="21"/>
-      <c r="V13" s="45" t="s">
+      <c r="V13" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="W13" s="46"/>
-      <c r="X13" s="46"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
       <c r="Y13" s="22"/>
       <c r="Z13" s="22"/>
       <c r="AA13" s="21"/>
     </row>
-    <row r="14" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B14" s="20"/>
       <c r="C14" s="28">
         <v>0.5</v>
@@ -4826,18 +4840,18 @@
       <c r="E14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
-      <c r="I14" s="54" t="s">
+      <c r="I14" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="56"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="54"/>
       <c r="M14" s="21"/>
-      <c r="O14" s="45" t="s">
+      <c r="O14" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
       <c r="T14" s="21"/>
@@ -4918,7 +4932,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B16" s="20"/>
       <c r="C16" s="28">
         <v>1</v>
@@ -4948,7 +4962,7 @@
       </c>
       <c r="Q16" s="22">
         <f>(180/PI())*(-ACOS(SQRT(G8^2+H8^2)*Q15/(3*Q6*Q7)+Q7*COS(-ATAN(H8/G8))/Q6)+ATAN(H8/G8))</f>
-        <v>8.0519364541616358</v>
+        <v>12.763351225118452</v>
       </c>
       <c r="R16" s="22" t="s">
         <v>83</v>
@@ -4956,7 +4970,7 @@
       <c r="S16" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="T16" s="61" t="s">
+      <c r="T16" s="33" t="s">
         <v>92</v>
       </c>
       <c r="V16" s="20" t="s">
@@ -5007,7 +5021,7 @@
       <c r="Z17" s="22"/>
       <c r="AA17" s="21"/>
     </row>
-    <row r="18" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B18" s="20"/>
       <c r="C18" s="28">
         <v>1.5</v>
@@ -5024,19 +5038,19 @@
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="45" t="s">
+      <c r="O18" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="21"/>
-      <c r="V18" s="45" t="s">
+      <c r="V18" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="W18" s="46"/>
-      <c r="X18" s="46"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
       <c r="AA18" s="21"/>
@@ -5066,7 +5080,7 @@
       </c>
       <c r="Q19" s="27">
         <f>(-3*Q6*Q7*SIN(Q16*PI()/180-ATAN(H8/G8))+3*Q7*Q7*SIN(-ATAN(H8/G8)))/SQRT(G8^2+H8^2)</f>
-        <v>164310.41127272265</v>
+        <v>342800.12071209063</v>
       </c>
       <c r="R19" s="22" t="s">
         <v>95</v>
@@ -5097,7 +5111,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B20" s="20"/>
       <c r="C20" s="28">
         <v>2</v>
@@ -5122,7 +5136,7 @@
       </c>
       <c r="Q20" s="22">
         <f>Q15/SQRT(Q15^2+Q19^2)</f>
-        <v>0.76471816467433307</v>
+        <v>0.49444485276290151</v>
       </c>
       <c r="R20" s="22"/>
       <c r="S20" s="22" t="s">
@@ -5138,8 +5152,8 @@
         <v>78</v>
       </c>
       <c r="X20" s="22">
-        <f>(180/PI())*(-ACOS(SQRT(G8^2+H8^2)*X19/(3*X6*X10)+X10*COS(-ATAN(H8/G8))/X6)+ATAN(H8/G8))</f>
-        <v>10.591744642816032</v>
+        <f>(180/PI())*(-ACOS(SQRT(G8^2+H8^2)*X19/(3*X6*X11)+X11*COS(-ATAN(H8/G8))/X6)+ATAN(H8/G8))</f>
+        <v>17.303936133609461</v>
       </c>
       <c r="Y20" s="22" t="s">
         <v>83</v>
@@ -5176,7 +5190,7 @@
       </c>
       <c r="Q21" s="22">
         <f>SQRT(Q15^2+Q19^2)/(SQRT(3)*D8)</f>
-        <v>669.19070017432409</v>
+        <v>1034.9835400143888</v>
       </c>
       <c r="R21" s="22" t="s">
         <v>84</v>
@@ -5194,7 +5208,7 @@
       <c r="Z21" s="22"/>
       <c r="AA21" s="21"/>
     </row>
-    <row r="22" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B22" s="20"/>
       <c r="C22" s="28">
         <v>2.5</v>
@@ -5209,7 +5223,10 @@
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
+      <c r="L22" s="22">
+        <f>(G8^2+H8^2)</f>
+        <v>1.7833000000000002E-2</v>
+      </c>
       <c r="M22" s="21"/>
       <c r="O22" s="20" t="s">
         <v>65</v>
@@ -5219,7 +5236,7 @@
       </c>
       <c r="Q22" s="22">
         <f>ACOS(Q20)*180/PI()</f>
-        <v>40.118074788615502</v>
+        <v>60.366850038261049</v>
       </c>
       <c r="R22" s="22" t="s">
         <v>83</v>
@@ -5230,11 +5247,11 @@
       <c r="T22" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="V22" s="45" t="s">
+      <c r="V22" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="W22" s="46"/>
-      <c r="X22" s="46"/>
+      <c r="W22" s="49"/>
+      <c r="X22" s="49"/>
       <c r="Y22" s="22"/>
       <c r="Z22" s="22"/>
       <c r="AA22" s="21"/>
@@ -5278,12 +5295,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="O24" s="45" t="s">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="O24" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
       <c r="T24" s="21"/>
@@ -5345,7 +5362,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
       <c r="O26" s="20" t="s">
         <v>63</v>
       </c>
@@ -5354,7 +5371,7 @@
       </c>
       <c r="Q26" s="27">
         <f>L16-Q19</f>
-        <v>-14310.411272722646</v>
+        <v>-192800.12071209063</v>
       </c>
       <c r="R26" s="22" t="s">
         <v>95</v>
@@ -5394,7 +5411,7 @@
       </c>
       <c r="Q27" s="27">
         <f>SQRT(Q25^2+Q26^2)</f>
-        <v>56831.222675519377</v>
+        <v>200491.61216020165</v>
       </c>
       <c r="R27" s="22" t="s">
         <v>85</v>
@@ -5412,7 +5429,7 @@
       <c r="Z27" s="22"/>
       <c r="AA27" s="21"/>
     </row>
-    <row r="28" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
       <c r="O28" s="20" t="s">
         <v>65</v>
       </c>
@@ -5421,7 +5438,7 @@
       </c>
       <c r="Q28" s="22">
         <f>Q25/Q27</f>
-        <v>0.96777787650329417</v>
+        <v>0.27432569077280189</v>
       </c>
       <c r="R28" s="22"/>
       <c r="S28" s="22" t="s">
@@ -5430,11 +5447,11 @@
       <c r="T28" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="V28" s="45" t="s">
+      <c r="V28" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="W28" s="46"/>
-      <c r="X28" s="46"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
       <c r="Y28" s="22"/>
       <c r="Z28" s="22"/>
       <c r="AA28" s="21"/>
@@ -5465,12 +5482,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="2:27" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="O30" s="45" t="s">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="O30" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
       <c r="R30" s="22"/>
       <c r="S30" s="22"/>
       <c r="T30" s="21"/>
@@ -5502,7 +5519,7 @@
       </c>
       <c r="Q31" s="22">
         <f>Q6*COS(Q16*PI()/180)</f>
-        <v>256.65649196859414</v>
+        <v>252.80702882214877</v>
       </c>
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
@@ -5535,7 +5552,7 @@
       </c>
       <c r="Q32" s="22">
         <f>Q6*SIN(Q16*PI()/180)</f>
-        <v>36.307992522314166</v>
+        <v>57.266319671711834</v>
       </c>
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
@@ -5571,20 +5588,20 @@
       <c r="Z33" s="22"/>
       <c r="AA33" s="21"/>
     </row>
-    <row r="34" spans="15:27" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="O34" s="45" t="s">
+    <row r="34" spans="15:27" x14ac:dyDescent="0.2">
+      <c r="O34" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="P34" s="46"/>
-      <c r="Q34" s="46"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
       <c r="R34" s="22"/>
       <c r="S34" s="22"/>
       <c r="T34" s="21"/>
-      <c r="V34" s="45" t="s">
+      <c r="V34" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="W34" s="46"/>
-      <c r="X34" s="46"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
       <c r="Y34" s="22"/>
       <c r="Z34" s="22"/>
       <c r="AA34" s="21"/>
@@ -5626,7 +5643,7 @@
       </c>
       <c r="Q36" s="22">
         <f>Q21*G8*SIN(-Q22*PI()/180)</f>
-        <v>-5.1744360097617026</v>
+        <v>-10.795404107528826</v>
       </c>
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
@@ -5659,20 +5676,20 @@
       <c r="Z37" s="22"/>
       <c r="AA37" s="21"/>
     </row>
-    <row r="38" spans="15:27" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="O38" s="45" t="s">
+    <row r="38" spans="15:27" x14ac:dyDescent="0.2">
+      <c r="O38" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="P38" s="46"/>
-      <c r="Q38" s="46"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
       <c r="T38" s="21"/>
-      <c r="V38" s="45" t="s">
+      <c r="V38" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="W38" s="46"/>
-      <c r="X38" s="46"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49"/>
       <c r="Y38" s="22"/>
       <c r="Z38" s="22"/>
       <c r="AA38" s="21"/>
@@ -5686,7 +5703,7 @@
       </c>
       <c r="Q39" s="22">
         <f>Q21*H8*COS(PI()/2-Q22*PI()/180)</f>
-        <v>57.349999108192215</v>
+        <v>119.64906219177783</v>
       </c>
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
@@ -5747,20 +5764,20 @@
       <c r="Z41" s="22"/>
       <c r="AA41" s="21"/>
     </row>
-    <row r="42" spans="15:27" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="O42" s="45" t="s">
+    <row r="42" spans="15:27" x14ac:dyDescent="0.2">
+      <c r="O42" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="P42" s="46"/>
-      <c r="Q42" s="46"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
       <c r="T42" s="21"/>
-      <c r="V42" s="45" t="s">
+      <c r="V42" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="W42" s="46"/>
-      <c r="X42" s="46"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
       <c r="Y42" s="22"/>
       <c r="Z42" s="22"/>
       <c r="AA42" s="21"/>
@@ -5774,7 +5791,7 @@
       </c>
       <c r="Q43" s="22">
         <f>Q7</f>
-        <v>220</v>
+        <v>127.01705922171767</v>
       </c>
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
@@ -5828,12 +5845,12 @@
       <c r="Z45" s="22"/>
       <c r="AA45" s="21"/>
     </row>
-    <row r="46" spans="15:27" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="V46" s="45" t="s">
+    <row r="46" spans="15:27" x14ac:dyDescent="0.2">
+      <c r="V46" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="W46" s="46"/>
-      <c r="X46" s="46"/>
+      <c r="W46" s="49"/>
+      <c r="X46" s="49"/>
       <c r="Y46" s="22"/>
       <c r="Z46" s="22"/>
       <c r="AA46" s="21"/>
@@ -5869,6 +5886,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="V34:X34"/>
+    <mergeCell ref="V38:X38"/>
+    <mergeCell ref="V42:X42"/>
+    <mergeCell ref="V46:X46"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O42:Q42"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="V2:AA2"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="V22:X22"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="O9:Q9"/>
@@ -5881,23 +5915,6 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="C5:L5"/>
-    <mergeCell ref="V2:AA2"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="V18:X18"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="O42:Q42"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="V34:X34"/>
-    <mergeCell ref="V38:X38"/>
-    <mergeCell ref="V42:X42"/>
-    <mergeCell ref="V46:X46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>